<commit_message>
flow use case, assignment
</commit_message>
<xml_diff>
--- a/Assignment.xlsx
+++ b/Assignment.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>Name</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>week12</t>
+  </si>
+  <si>
+    <t>week13</t>
+  </si>
+  <si>
+    <t>Hoàn thiện tài liệu</t>
   </si>
 </sst>
 </file>
@@ -429,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:N5"/>
+  <dimension ref="B3:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,7 +454,7 @@
     <col min="14" max="14" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -488,8 +494,11 @@
       <c r="N3" t="s">
         <v>30</v>
       </c>
+      <c r="O3" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -529,8 +538,11 @@
       <c r="N4" t="s">
         <v>26</v>
       </c>
+      <c r="O4" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>

</xml_diff>